<commit_message>
- Kommentare in NNPlayer2 eingefügt. - Auswertung 4 x 5
</commit_message>
<xml_diff>
--- a/Sicherung/NN200P2/Test NN DS200.xlsx
+++ b/Sicherung/NN200P2/Test NN DS200.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18514" windowHeight="7971" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18514" windowHeight="7971"/>
   </bookViews>
   <sheets>
     <sheet name="abwechselnd" sheetId="1" r:id="rId1"/>
@@ -180,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -195,8 +195,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -210,11 +210,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -227,6 +227,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -544,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10:H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -653,27 +668,27 @@
       <c r="A10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="14">
         <v>30</v>
       </c>
       <c r="C10" s="2">
         <v>2713</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="19">
         <f>AVERAGE(C10:C14)</f>
         <v>2694.4</v>
       </c>
       <c r="E10" s="2">
         <v>0</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="14">
         <f>AVERAGE(E10:E14)</f>
         <v>0</v>
       </c>
       <c r="G10" s="2">
         <v>7287</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="19">
         <f>AVERAGE(G10:G14)</f>
         <v>7305.6</v>
       </c>
@@ -684,19 +699,19 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" s="15"/>
-      <c r="B11" s="13"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="2">
         <v>2680</v>
       </c>
-      <c r="D11" s="13"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="2">
         <v>0</v>
       </c>
-      <c r="F11" s="13"/>
+      <c r="F11" s="14"/>
       <c r="G11" s="2">
         <v>7320</v>
       </c>
-      <c r="H11" s="13"/>
+      <c r="H11" s="19"/>
       <c r="I11">
         <f t="shared" ref="I11:I34" si="0">SUM(C11,E11,G11)</f>
         <v>10000</v>
@@ -704,19 +719,19 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="15"/>
-      <c r="B12" s="13"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="2">
         <v>2716</v>
       </c>
-      <c r="D12" s="13"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="2">
         <v>0</v>
       </c>
-      <c r="F12" s="13"/>
+      <c r="F12" s="14"/>
       <c r="G12" s="2">
         <v>7284</v>
       </c>
-      <c r="H12" s="13"/>
+      <c r="H12" s="19"/>
       <c r="I12">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -724,19 +739,19 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" s="15"/>
-      <c r="B13" s="13"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="2">
         <v>2685</v>
       </c>
-      <c r="D13" s="13"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="2">
         <v>0</v>
       </c>
-      <c r="F13" s="13"/>
+      <c r="F13" s="14"/>
       <c r="G13" s="2">
         <v>7315</v>
       </c>
-      <c r="H13" s="13"/>
+      <c r="H13" s="19"/>
       <c r="I13">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -744,19 +759,19 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" s="15"/>
-      <c r="B14" s="13"/>
+      <c r="B14" s="14"/>
       <c r="C14" s="2">
         <v>2678</v>
       </c>
-      <c r="D14" s="13"/>
+      <c r="D14" s="19"/>
       <c r="E14" s="2">
         <v>0</v>
       </c>
-      <c r="F14" s="13"/>
+      <c r="F14" s="14"/>
       <c r="G14" s="2">
         <v>7322</v>
       </c>
-      <c r="H14" s="13"/>
+      <c r="H14" s="19"/>
       <c r="I14">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -766,27 +781,27 @@
       <c r="A15" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="13">
         <v>60</v>
       </c>
       <c r="C15" s="3">
         <v>1710</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="20">
         <f>AVERAGE(C15:C19)</f>
         <v>1701.6</v>
       </c>
       <c r="E15" s="3">
         <v>0</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="13">
         <f t="shared" ref="F15" si="1">AVERAGE(E15:E19)</f>
         <v>0</v>
       </c>
       <c r="G15" s="3">
         <v>8290</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="20">
         <f t="shared" ref="H15" si="2">AVERAGE(G15:G19)</f>
         <v>8298.4</v>
       </c>
@@ -797,19 +812,19 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="16"/>
-      <c r="B16" s="8"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="3">
         <v>1688</v>
       </c>
-      <c r="D16" s="8"/>
+      <c r="D16" s="20"/>
       <c r="E16" s="3">
         <v>0</v>
       </c>
-      <c r="F16" s="8"/>
+      <c r="F16" s="13"/>
       <c r="G16" s="3">
         <v>8312</v>
       </c>
-      <c r="H16" s="8"/>
+      <c r="H16" s="20"/>
       <c r="I16">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -817,19 +832,19 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="16"/>
-      <c r="B17" s="8"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="4">
         <v>1703</v>
       </c>
-      <c r="D17" s="8"/>
+      <c r="D17" s="20"/>
       <c r="E17" s="4">
         <v>0</v>
       </c>
-      <c r="F17" s="8"/>
+      <c r="F17" s="13"/>
       <c r="G17" s="4">
         <v>8297</v>
       </c>
-      <c r="H17" s="8"/>
+      <c r="H17" s="20"/>
       <c r="I17">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -837,19 +852,19 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="16"/>
-      <c r="B18" s="8"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="4">
         <v>1689</v>
       </c>
-      <c r="D18" s="8"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="4">
         <v>0</v>
       </c>
-      <c r="F18" s="8"/>
+      <c r="F18" s="13"/>
       <c r="G18" s="4">
         <v>8311</v>
       </c>
-      <c r="H18" s="8"/>
+      <c r="H18" s="20"/>
       <c r="I18">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -857,19 +872,19 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="16"/>
-      <c r="B19" s="8"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="4">
         <v>1718</v>
       </c>
-      <c r="D19" s="8"/>
+      <c r="D19" s="20"/>
       <c r="E19" s="4">
         <v>0</v>
       </c>
-      <c r="F19" s="8"/>
+      <c r="F19" s="13"/>
       <c r="G19" s="4">
         <v>8282</v>
       </c>
-      <c r="H19" s="8"/>
+      <c r="H19" s="20"/>
       <c r="I19">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -885,7 +900,7 @@
       <c r="C20" s="5">
         <v>3323</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="21">
         <f t="shared" ref="D20" si="3">AVERAGE(C20:C24)</f>
         <v>3292.2</v>
       </c>
@@ -899,7 +914,7 @@
       <c r="G20" s="5">
         <v>6677</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="21">
         <f t="shared" ref="H20" si="5">AVERAGE(G20:G24)</f>
         <v>6707.8</v>
       </c>
@@ -914,7 +929,7 @@
       <c r="C21" s="5">
         <v>3298</v>
       </c>
-      <c r="D21" s="9"/>
+      <c r="D21" s="21"/>
       <c r="E21" s="5">
         <v>0</v>
       </c>
@@ -922,7 +937,7 @@
       <c r="G21" s="5">
         <v>6702</v>
       </c>
-      <c r="H21" s="9"/>
+      <c r="H21" s="21"/>
       <c r="I21">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -934,7 +949,7 @@
       <c r="C22" s="5">
         <v>3280</v>
       </c>
-      <c r="D22" s="9"/>
+      <c r="D22" s="21"/>
       <c r="E22" s="5">
         <v>0</v>
       </c>
@@ -942,7 +957,7 @@
       <c r="G22" s="5">
         <v>6720</v>
       </c>
-      <c r="H22" s="9"/>
+      <c r="H22" s="21"/>
       <c r="I22">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -954,7 +969,7 @@
       <c r="C23" s="5">
         <v>3310</v>
       </c>
-      <c r="D23" s="9"/>
+      <c r="D23" s="21"/>
       <c r="E23" s="5">
         <v>0</v>
       </c>
@@ -962,7 +977,7 @@
       <c r="G23" s="5">
         <v>6690</v>
       </c>
-      <c r="H23" s="9"/>
+      <c r="H23" s="21"/>
       <c r="I23">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -974,7 +989,7 @@
       <c r="C24" s="5">
         <v>3250</v>
       </c>
-      <c r="D24" s="9"/>
+      <c r="D24" s="21"/>
       <c r="E24" s="5">
         <v>0</v>
       </c>
@@ -982,7 +997,7 @@
       <c r="G24" s="5">
         <v>6750</v>
       </c>
-      <c r="H24" s="9"/>
+      <c r="H24" s="21"/>
       <c r="I24">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -998,7 +1013,7 @@
       <c r="C25" s="6">
         <v>2534</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="22">
         <f t="shared" ref="D25" si="6">AVERAGE(C25:C29)</f>
         <v>2591.4</v>
       </c>
@@ -1012,7 +1027,7 @@
       <c r="G25" s="6">
         <v>7466</v>
       </c>
-      <c r="H25" s="10">
+      <c r="H25" s="22">
         <f t="shared" ref="H25" si="8">AVERAGE(G25:G29)</f>
         <v>7408.6</v>
       </c>
@@ -1027,7 +1042,7 @@
       <c r="C26" s="6">
         <v>2579</v>
       </c>
-      <c r="D26" s="10"/>
+      <c r="D26" s="22"/>
       <c r="E26" s="6">
         <v>0</v>
       </c>
@@ -1035,7 +1050,7 @@
       <c r="G26" s="6">
         <v>7421</v>
       </c>
-      <c r="H26" s="10"/>
+      <c r="H26" s="22"/>
       <c r="I26">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -1047,7 +1062,7 @@
       <c r="C27" s="6">
         <v>2620</v>
       </c>
-      <c r="D27" s="10"/>
+      <c r="D27" s="22"/>
       <c r="E27" s="6">
         <v>0</v>
       </c>
@@ -1055,7 +1070,7 @@
       <c r="G27" s="6">
         <v>7380</v>
       </c>
-      <c r="H27" s="10"/>
+      <c r="H27" s="22"/>
       <c r="I27">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -1067,7 +1082,7 @@
       <c r="C28" s="6">
         <v>2617</v>
       </c>
-      <c r="D28" s="10"/>
+      <c r="D28" s="22"/>
       <c r="E28" s="6">
         <v>0</v>
       </c>
@@ -1075,7 +1090,7 @@
       <c r="G28" s="6">
         <v>7383</v>
       </c>
-      <c r="H28" s="10"/>
+      <c r="H28" s="22"/>
       <c r="I28">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -1087,7 +1102,7 @@
       <c r="C29" s="6">
         <v>2607</v>
       </c>
-      <c r="D29" s="10"/>
+      <c r="D29" s="22"/>
       <c r="E29" s="6">
         <v>0</v>
       </c>
@@ -1095,14 +1110,14 @@
       <c r="G29" s="6">
         <v>7393</v>
       </c>
-      <c r="H29" s="10"/>
+      <c r="H29" s="22"/>
       <c r="I29">
         <f t="shared" si="0"/>
         <v>10000</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B30" s="11">
@@ -1111,7 +1126,7 @@
       <c r="C30" s="7">
         <v>1798</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D30" s="23">
         <f t="shared" ref="D30" si="9">AVERAGE(C30:C34)</f>
         <v>1788.8</v>
       </c>
@@ -1125,7 +1140,7 @@
       <c r="G30" s="7">
         <v>8202</v>
       </c>
-      <c r="H30" s="11">
+      <c r="H30" s="23">
         <f t="shared" ref="H30" si="10">AVERAGE(G30:G34)</f>
         <v>8211.2000000000007</v>
       </c>
@@ -1135,12 +1150,12 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A31" s="14"/>
+      <c r="A31" s="8"/>
       <c r="B31" s="11"/>
       <c r="C31" s="7">
         <v>1778</v>
       </c>
-      <c r="D31" s="11"/>
+      <c r="D31" s="23"/>
       <c r="E31" s="7">
         <v>0</v>
       </c>
@@ -1148,19 +1163,19 @@
       <c r="G31" s="7">
         <v>8222</v>
       </c>
-      <c r="H31" s="11"/>
+      <c r="H31" s="23"/>
       <c r="I31">
         <f t="shared" si="0"/>
         <v>10000</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A32" s="14"/>
+      <c r="A32" s="8"/>
       <c r="B32" s="11"/>
       <c r="C32" s="7">
         <v>1820</v>
       </c>
-      <c r="D32" s="11"/>
+      <c r="D32" s="23"/>
       <c r="E32" s="7">
         <v>0</v>
       </c>
@@ -1168,19 +1183,19 @@
       <c r="G32" s="7">
         <v>8180</v>
       </c>
-      <c r="H32" s="11"/>
+      <c r="H32" s="23"/>
       <c r="I32">
         <f>SUM(C32,E32,G32)</f>
         <v>10000</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A33" s="14"/>
+      <c r="A33" s="8"/>
       <c r="B33" s="11"/>
       <c r="C33" s="7">
         <v>1770</v>
       </c>
-      <c r="D33" s="11"/>
+      <c r="D33" s="23"/>
       <c r="E33" s="7">
         <v>0</v>
       </c>
@@ -1188,19 +1203,19 @@
       <c r="G33" s="7">
         <v>8230</v>
       </c>
-      <c r="H33" s="11"/>
+      <c r="H33" s="23"/>
       <c r="I33">
         <f t="shared" si="0"/>
         <v>10000</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A34" s="14"/>
+      <c r="A34" s="8"/>
       <c r="B34" s="11"/>
       <c r="C34" s="7">
         <v>1778</v>
       </c>
-      <c r="D34" s="11"/>
+      <c r="D34" s="23"/>
       <c r="E34" s="7">
         <v>0</v>
       </c>
@@ -1208,7 +1223,7 @@
       <c r="G34" s="7">
         <v>8222</v>
       </c>
-      <c r="H34" s="11"/>
+      <c r="H34" s="23"/>
       <c r="I34">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -1216,6 +1231,21 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="F15:F19"/>
+    <mergeCell ref="F20:F24"/>
+    <mergeCell ref="F25:F29"/>
+    <mergeCell ref="F30:F34"/>
+    <mergeCell ref="H15:H19"/>
+    <mergeCell ref="H20:H24"/>
+    <mergeCell ref="H25:H29"/>
+    <mergeCell ref="H30:H34"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="D10:D14"/>
+    <mergeCell ref="F10:F14"/>
+    <mergeCell ref="H10:H14"/>
+    <mergeCell ref="E8:F8"/>
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="B20:B24"/>
     <mergeCell ref="B25:B29"/>
@@ -1231,21 +1261,6 @@
     <mergeCell ref="A15:A19"/>
     <mergeCell ref="A20:A24"/>
     <mergeCell ref="A25:A29"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="D10:D14"/>
-    <mergeCell ref="F10:F14"/>
-    <mergeCell ref="H10:H14"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="F15:F19"/>
-    <mergeCell ref="F20:F24"/>
-    <mergeCell ref="F25:F29"/>
-    <mergeCell ref="F30:F34"/>
-    <mergeCell ref="H15:H19"/>
-    <mergeCell ref="H20:H24"/>
-    <mergeCell ref="H25:H29"/>
-    <mergeCell ref="H30:H34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1255,8 +1270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10:H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1364,27 +1379,27 @@
       <c r="A10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="14">
         <v>30</v>
       </c>
       <c r="C10" s="2">
         <v>3919</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="19">
         <f>AVERAGE(C10:C14)</f>
         <v>3920</v>
       </c>
       <c r="E10" s="2">
         <v>0</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="14">
         <f>AVERAGE(E10:E14)</f>
         <v>0</v>
       </c>
       <c r="G10" s="2">
         <v>6081</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="19">
         <f>AVERAGE(G10:G14)</f>
         <v>6080</v>
       </c>
@@ -1395,19 +1410,19 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" s="15"/>
-      <c r="B11" s="13"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="2">
         <v>3870</v>
       </c>
-      <c r="D11" s="13"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="2">
         <v>0</v>
       </c>
-      <c r="F11" s="13"/>
+      <c r="F11" s="14"/>
       <c r="G11" s="2">
         <v>6130</v>
       </c>
-      <c r="H11" s="13"/>
+      <c r="H11" s="19"/>
       <c r="I11">
         <f t="shared" ref="I11:I34" si="0">SUM(C11,E11,G11)</f>
         <v>10000</v>
@@ -1415,19 +1430,19 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="15"/>
-      <c r="B12" s="13"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="2">
         <v>3957</v>
       </c>
-      <c r="D12" s="13"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="2">
         <v>0</v>
       </c>
-      <c r="F12" s="13"/>
+      <c r="F12" s="14"/>
       <c r="G12" s="2">
         <v>6043</v>
       </c>
-      <c r="H12" s="13"/>
+      <c r="H12" s="19"/>
       <c r="I12">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -1435,19 +1450,19 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" s="15"/>
-      <c r="B13" s="13"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="2">
         <v>3905</v>
       </c>
-      <c r="D13" s="13"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="2">
         <v>0</v>
       </c>
-      <c r="F13" s="13"/>
+      <c r="F13" s="14"/>
       <c r="G13" s="2">
         <v>6095</v>
       </c>
-      <c r="H13" s="13"/>
+      <c r="H13" s="19"/>
       <c r="I13">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -1455,19 +1470,19 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" s="15"/>
-      <c r="B14" s="13"/>
+      <c r="B14" s="14"/>
       <c r="C14" s="2">
         <v>3949</v>
       </c>
-      <c r="D14" s="13"/>
+      <c r="D14" s="19"/>
       <c r="E14" s="2">
         <v>0</v>
       </c>
-      <c r="F14" s="13"/>
+      <c r="F14" s="14"/>
       <c r="G14" s="2">
         <v>6051</v>
       </c>
-      <c r="H14" s="13"/>
+      <c r="H14" s="19"/>
       <c r="I14">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -1477,27 +1492,27 @@
       <c r="A15" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="13">
         <v>60</v>
       </c>
       <c r="C15" s="3">
         <v>3387</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="20">
         <f>AVERAGE(C15:C19)</f>
         <v>3369.4</v>
       </c>
       <c r="E15" s="3">
         <v>0</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="13">
         <f t="shared" ref="F15" si="1">AVERAGE(E15:E19)</f>
         <v>0</v>
       </c>
       <c r="G15" s="3">
         <v>6613</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="20">
         <f t="shared" ref="H15" si="2">AVERAGE(G15:G19)</f>
         <v>6630.6</v>
       </c>
@@ -1508,19 +1523,19 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="16"/>
-      <c r="B16" s="8"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="3">
         <v>3449</v>
       </c>
-      <c r="D16" s="8"/>
+      <c r="D16" s="20"/>
       <c r="E16" s="3">
         <v>0</v>
       </c>
-      <c r="F16" s="8"/>
+      <c r="F16" s="13"/>
       <c r="G16" s="3">
         <v>6551</v>
       </c>
-      <c r="H16" s="8"/>
+      <c r="H16" s="20"/>
       <c r="I16">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -1528,19 +1543,19 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="16"/>
-      <c r="B17" s="8"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="4">
         <v>3337</v>
       </c>
-      <c r="D17" s="8"/>
+      <c r="D17" s="20"/>
       <c r="E17" s="4">
         <v>0</v>
       </c>
-      <c r="F17" s="8"/>
+      <c r="F17" s="13"/>
       <c r="G17" s="4">
         <v>6663</v>
       </c>
-      <c r="H17" s="8"/>
+      <c r="H17" s="20"/>
       <c r="I17">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -1548,19 +1563,19 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="16"/>
-      <c r="B18" s="8"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="4">
         <v>3331</v>
       </c>
-      <c r="D18" s="8"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="4">
         <v>0</v>
       </c>
-      <c r="F18" s="8"/>
+      <c r="F18" s="13"/>
       <c r="G18" s="4">
         <v>6669</v>
       </c>
-      <c r="H18" s="8"/>
+      <c r="H18" s="20"/>
       <c r="I18">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -1568,19 +1583,19 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="16"/>
-      <c r="B19" s="8"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="4">
         <v>3343</v>
       </c>
-      <c r="D19" s="8"/>
+      <c r="D19" s="20"/>
       <c r="E19" s="4">
         <v>0</v>
       </c>
-      <c r="F19" s="8"/>
+      <c r="F19" s="13"/>
       <c r="G19" s="4">
         <v>6657</v>
       </c>
-      <c r="H19" s="8"/>
+      <c r="H19" s="20"/>
       <c r="I19">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -1596,7 +1611,7 @@
       <c r="C20" s="5">
         <v>3425</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="21">
         <f t="shared" ref="D20" si="3">AVERAGE(C20:C24)</f>
         <v>3468.6</v>
       </c>
@@ -1610,7 +1625,7 @@
       <c r="G20" s="5">
         <v>6575</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="21">
         <f t="shared" ref="H20" si="5">AVERAGE(G20:G24)</f>
         <v>6531.4</v>
       </c>
@@ -1625,7 +1640,7 @@
       <c r="C21" s="5">
         <v>3430</v>
       </c>
-      <c r="D21" s="9"/>
+      <c r="D21" s="21"/>
       <c r="E21" s="5">
         <v>0</v>
       </c>
@@ -1633,7 +1648,7 @@
       <c r="G21" s="5">
         <v>6570</v>
       </c>
-      <c r="H21" s="9"/>
+      <c r="H21" s="21"/>
       <c r="I21">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -1645,7 +1660,7 @@
       <c r="C22" s="5">
         <v>3552</v>
       </c>
-      <c r="D22" s="9"/>
+      <c r="D22" s="21"/>
       <c r="E22" s="5">
         <v>0</v>
       </c>
@@ -1653,7 +1668,7 @@
       <c r="G22" s="5">
         <v>6448</v>
       </c>
-      <c r="H22" s="9"/>
+      <c r="H22" s="21"/>
       <c r="I22">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -1665,7 +1680,7 @@
       <c r="C23" s="5">
         <v>3525</v>
       </c>
-      <c r="D23" s="9"/>
+      <c r="D23" s="21"/>
       <c r="E23" s="5">
         <v>0</v>
       </c>
@@ -1673,7 +1688,7 @@
       <c r="G23" s="5">
         <v>6475</v>
       </c>
-      <c r="H23" s="9"/>
+      <c r="H23" s="21"/>
       <c r="I23">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -1685,7 +1700,7 @@
       <c r="C24" s="5">
         <v>3411</v>
       </c>
-      <c r="D24" s="9"/>
+      <c r="D24" s="21"/>
       <c r="E24" s="5">
         <v>0</v>
       </c>
@@ -1693,7 +1708,7 @@
       <c r="G24" s="5">
         <v>6589</v>
       </c>
-      <c r="H24" s="9"/>
+      <c r="H24" s="21"/>
       <c r="I24">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -1709,7 +1724,7 @@
       <c r="C25" s="6">
         <v>3925</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="22">
         <f t="shared" ref="D25" si="6">AVERAGE(C25:C29)</f>
         <v>3947.4</v>
       </c>
@@ -1723,7 +1738,7 @@
       <c r="G25" s="6">
         <v>6075</v>
       </c>
-      <c r="H25" s="10">
+      <c r="H25" s="22">
         <f t="shared" ref="H25" si="8">AVERAGE(G25:G29)</f>
         <v>6052.6</v>
       </c>
@@ -1738,7 +1753,7 @@
       <c r="C26" s="6">
         <v>3890</v>
       </c>
-      <c r="D26" s="10"/>
+      <c r="D26" s="22"/>
       <c r="E26" s="6">
         <v>0</v>
       </c>
@@ -1746,7 +1761,7 @@
       <c r="G26" s="6">
         <v>6110</v>
       </c>
-      <c r="H26" s="10"/>
+      <c r="H26" s="22"/>
       <c r="I26">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -1758,7 +1773,7 @@
       <c r="C27" s="6">
         <v>3967</v>
       </c>
-      <c r="D27" s="10"/>
+      <c r="D27" s="22"/>
       <c r="E27" s="6">
         <v>0</v>
       </c>
@@ -1766,7 +1781,7 @@
       <c r="G27" s="6">
         <v>6033</v>
       </c>
-      <c r="H27" s="10"/>
+      <c r="H27" s="22"/>
       <c r="I27">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -1778,7 +1793,7 @@
       <c r="C28" s="6">
         <v>3977</v>
       </c>
-      <c r="D28" s="10"/>
+      <c r="D28" s="22"/>
       <c r="E28" s="6">
         <v>0</v>
       </c>
@@ -1786,7 +1801,7 @@
       <c r="G28" s="6">
         <v>6023</v>
       </c>
-      <c r="H28" s="10"/>
+      <c r="H28" s="22"/>
       <c r="I28">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -1798,7 +1813,7 @@
       <c r="C29" s="6">
         <v>3978</v>
       </c>
-      <c r="D29" s="10"/>
+      <c r="D29" s="22"/>
       <c r="E29" s="6">
         <v>0</v>
       </c>
@@ -1806,14 +1821,14 @@
       <c r="G29" s="6">
         <v>6022</v>
       </c>
-      <c r="H29" s="10"/>
+      <c r="H29" s="22"/>
       <c r="I29">
         <f t="shared" si="0"/>
         <v>10000</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B30" s="11">
@@ -1822,7 +1837,7 @@
       <c r="C30" s="7">
         <v>3517</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D30" s="23">
         <f t="shared" ref="D30" si="9">AVERAGE(C30:C34)</f>
         <v>3550.6</v>
       </c>
@@ -1836,7 +1851,7 @@
       <c r="G30" s="7">
         <v>6483</v>
       </c>
-      <c r="H30" s="11">
+      <c r="H30" s="23">
         <f t="shared" ref="H30" si="10">AVERAGE(G30:G34)</f>
         <v>6449.4</v>
       </c>
@@ -1846,12 +1861,12 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A31" s="14"/>
+      <c r="A31" s="8"/>
       <c r="B31" s="11"/>
       <c r="C31" s="7">
         <v>3499</v>
       </c>
-      <c r="D31" s="11"/>
+      <c r="D31" s="23"/>
       <c r="E31" s="7">
         <v>0</v>
       </c>
@@ -1859,19 +1874,19 @@
       <c r="G31" s="7">
         <v>6501</v>
       </c>
-      <c r="H31" s="11"/>
+      <c r="H31" s="23"/>
       <c r="I31">
         <f t="shared" si="0"/>
         <v>10000</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A32" s="14"/>
+      <c r="A32" s="8"/>
       <c r="B32" s="11"/>
       <c r="C32" s="7">
         <v>3649</v>
       </c>
-      <c r="D32" s="11"/>
+      <c r="D32" s="23"/>
       <c r="E32" s="7">
         <v>0</v>
       </c>
@@ -1879,19 +1894,19 @@
       <c r="G32" s="7">
         <v>6351</v>
       </c>
-      <c r="H32" s="11"/>
+      <c r="H32" s="23"/>
       <c r="I32">
         <f>SUM(C32,E32,G32)</f>
         <v>10000</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A33" s="14"/>
+      <c r="A33" s="8"/>
       <c r="B33" s="11"/>
       <c r="C33" s="7">
         <v>3548</v>
       </c>
-      <c r="D33" s="11"/>
+      <c r="D33" s="23"/>
       <c r="E33" s="7">
         <v>0</v>
       </c>
@@ -1899,19 +1914,19 @@
       <c r="G33" s="7">
         <v>6452</v>
       </c>
-      <c r="H33" s="11"/>
+      <c r="H33" s="23"/>
       <c r="I33">
         <f t="shared" si="0"/>
         <v>10000</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A34" s="14"/>
+      <c r="A34" s="8"/>
       <c r="B34" s="11"/>
       <c r="C34" s="7">
         <v>3540</v>
       </c>
-      <c r="D34" s="11"/>
+      <c r="D34" s="23"/>
       <c r="E34" s="7">
         <v>0</v>
       </c>
@@ -1919,7 +1934,7 @@
       <c r="G34" s="7">
         <v>6460</v>
       </c>
-      <c r="H34" s="11"/>
+      <c r="H34" s="23"/>
       <c r="I34">
         <f t="shared" si="0"/>
         <v>10000</v>
@@ -1927,36 +1942,36 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="D25:D29"/>
+    <mergeCell ref="F25:F29"/>
+    <mergeCell ref="H25:H29"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="B30:B34"/>
+    <mergeCell ref="D30:D34"/>
+    <mergeCell ref="F30:F34"/>
+    <mergeCell ref="H30:H34"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="D15:D19"/>
+    <mergeCell ref="F15:F19"/>
+    <mergeCell ref="H15:H19"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="D20:D24"/>
+    <mergeCell ref="F20:F24"/>
+    <mergeCell ref="H20:H24"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="D10:D14"/>
     <mergeCell ref="F10:F14"/>
     <mergeCell ref="H10:H14"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="D20:D24"/>
-    <mergeCell ref="F20:F24"/>
-    <mergeCell ref="H20:H24"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="D15:D19"/>
-    <mergeCell ref="F15:F19"/>
-    <mergeCell ref="H15:H19"/>
-    <mergeCell ref="A30:A34"/>
-    <mergeCell ref="B30:B34"/>
-    <mergeCell ref="D30:D34"/>
-    <mergeCell ref="F30:F34"/>
-    <mergeCell ref="H30:H34"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="B25:B29"/>
-    <mergeCell ref="D25:D29"/>
-    <mergeCell ref="F25:F29"/>
-    <mergeCell ref="H25:H29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>